<commit_message>
Added Extent Reports functionality
</commit_message>
<xml_diff>
--- a/TestNG/src/test/resources/testdata/ExcelFiles/LoginData.xlsx
+++ b/TestNG/src/test/resources/testdata/ExcelFiles/LoginData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programs\eclipse\web-automation-framework\TestNG\src\test\resources\testdata\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B872428-F4B0-400D-B5C1-00F0E01B6945}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FCDB4A8-BC62-4ADC-92A3-BC86250618F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>UserName</t>
   </si>
@@ -37,6 +37,9 @@
   </si>
   <si>
     <t>secret_sauce</t>
+  </si>
+  <si>
+    <t>locked_out_user</t>
   </si>
 </sst>
 </file>
@@ -86,9 +89,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -373,7 +375,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -383,26 +385,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>